<commit_message>
7 de marzo metodos 2.0
</commit_message>
<xml_diff>
--- a/Metodos numericos/parcial2/Newton Raphson.xlsx
+++ b/Metodos numericos/parcial2/Newton Raphson.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\OneDrive\Desktop\Sem4\Sem4ULSA\Metodos numericos\parcial2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA470722-AE46-4A70-8189-D0ECA6D3690C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2235F9CD-5F40-40A0-ADC3-3536F1066C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{721BABC6-5491-46A4-B4BA-3C4F68E5E618}"/>
   </bookViews>
@@ -187,7 +187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -212,14 +212,21 @@
     <xf numFmtId="10" fontId="0" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,8 +845,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2658,8 +2666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78077EB7-1996-48CF-939C-69F1030DF3FF}">
   <dimension ref="A2:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="110" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2930,272 +2938,325 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="4">
         <v>1</v>
       </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="A24" s="4">
         <f>SIN(SQRT(B21))-B21</f>
         <v>-0.1585290151921035</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="4">
         <f>-(SIN(SQRT(B21))/4*B21)-(COS(SQRT(B21))/(4*(B21^1.5)))</f>
         <v>-0.34544332266900907</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="4">
         <f>A24*B24</f>
         <v>5.4762789747406046E-2</v>
       </c>
-      <c r="F24" s="10">
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="4">
         <v>0</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G24" s="4">
         <f>SIN(SQRT(F24))-F24</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F25" s="10">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="4">
         <v>1</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25" s="4">
         <f t="shared" ref="G25:G34" si="4">SIN(SQRT(F25))-F25</f>
         <v>-0.1585290151921035</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="10">
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="4">
         <v>2</v>
       </c>
-      <c r="G26" s="10">
+      <c r="G26" s="4">
         <f t="shared" si="4"/>
         <v>-1.0122340540072643</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
+      <c r="A27" s="4">
         <v>0</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="4">
         <v>1</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="F27" s="10">
+      <c r="C27" s="4"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="4">
         <v>3</v>
       </c>
-      <c r="G27" s="10">
+      <c r="G27" s="4">
         <f t="shared" si="4"/>
         <v>-2.0129733550096462</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="A28" s="4">
         <v>1</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="4">
         <f>B27-(((SIN(SQRT(B27))-B27)/((COS(SQRT(B27)))/(2*(SQRT(B27)))-1)))</f>
         <v>0.78279199065750804</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="5">
         <f>(B28-B27)/B28</f>
         <v>-0.27747857915619134</v>
       </c>
-      <c r="F28" s="10">
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="4">
         <v>4</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="4">
         <f t="shared" si="4"/>
         <v>-3.0907025731743181</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
+      <c r="A29" s="4">
         <v>2</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="4">
         <f t="shared" ref="B29:B37" si="5">B28-(((SIN(SQRT(B28))-B28)/((COS(SQRT(B28)))/(2*(SQRT(B28)))-1)))</f>
         <v>0.76872356807973075</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="5">
         <f t="shared" ref="C29:C37" si="6">(B29-B28)/B29</f>
         <v>-1.8301016336626928E-2</v>
       </c>
-      <c r="F29" s="10">
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="4">
         <v>5</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29" s="4">
         <f t="shared" si="4"/>
         <v>-4.2132508684527856</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
+      <c r="A30" s="4">
         <v>3</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="4">
         <f t="shared" si="5"/>
         <v>0.76864885890174284</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="5">
         <f t="shared" si="6"/>
         <v>-9.7195458137612977E-5</v>
       </c>
-      <c r="F30" s="10">
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="4">
         <v>6</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G30" s="4">
         <f t="shared" si="4"/>
         <v>-5.3618423648515323</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="16">
+      <c r="A31" s="8">
         <v>4</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="8">
         <f t="shared" si="5"/>
         <v>0.76864885676094941</v>
       </c>
-      <c r="C31" s="17">
+      <c r="C31" s="9">
         <f t="shared" si="6"/>
         <v>-2.7851383796193918E-9</v>
       </c>
-      <c r="F31" s="10">
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="4">
         <v>7</v>
       </c>
-      <c r="G31" s="10">
+      <c r="G31" s="4">
         <f t="shared" si="4"/>
         <v>-6.5242281618472484</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
+      <c r="A32" s="4">
         <v>5</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="4">
         <f t="shared" si="5"/>
         <v>0.76864885676094941</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F32" s="10">
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="4">
         <v>8</v>
       </c>
-      <c r="G32" s="10">
+      <c r="G32" s="4">
         <f t="shared" si="4"/>
         <v>-7.6919282576369552</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
+      <c r="A33" s="4">
         <v>6</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="4">
         <f t="shared" si="5"/>
         <v>0.76864885676094941</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F33" s="10">
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="4">
         <v>9</v>
       </c>
-      <c r="G33" s="10">
+      <c r="G33" s="4">
         <f t="shared" si="4"/>
         <v>-8.8588799919401335</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
+      <c r="A34" s="4">
         <v>7</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="4">
         <f t="shared" si="5"/>
         <v>0.76864885676094941</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F34" s="10">
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="4">
         <v>10</v>
       </c>
-      <c r="G34" s="10">
+      <c r="G34" s="4">
         <f t="shared" si="4"/>
         <v>-10.020683531529583</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="10">
+      <c r="A35" s="4">
         <v>8</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B35" s="4">
         <f t="shared" si="5"/>
         <v>0.76864885676094941</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
+      <c r="A36" s="4">
         <v>9</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="4">
         <f t="shared" si="5"/>
         <v>0.76864885676094941</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="10">
+      <c r="A37" s="4">
         <v>10</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="4">
         <f t="shared" si="5"/>
         <v>0.76864885676094941</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>